<commit_message>
[FINAL] protein faas v2 [WILDCARD] The cool refreshing taste of Pepsi.
</commit_message>
<xml_diff>
--- a/comparative_func_analysis/report.xlsx
+++ b/comparative_func_analysis/report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uminho365-my.sharepoint.com/personal/id8006_uminho_pt/Documents/Papers/bit analysis/bit-analysis/comparative_func_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_2F9947B4C35C5CBE6410B4D55F5DCE3A8747BEF2" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D6D6C75F-6D88-4043-9617-4E1A32FF245D}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_24018149414BBABF6410B4D55F5DCE3A87478EFA" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9F98E864-3CF6-4E03-967E-2886B7948E80}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="309">
   <si>
     <t>name</t>
   </si>
@@ -76,7 +76,7 @@
     <t>ASM886v2</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/000/008/865/GCA_000008865.2_ASM886v2/GCA_000008865.2_ASM886v2_protein.faa.gz</t>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCF/000/008/865/GCF_000008865.2_ASM886v2/GCF_000008865.2_ASM886v2_protein.faa.gz</t>
   </si>
   <si>
     <t>Escherichia coli.faa.gz</t>
@@ -103,7 +103,7 @@
     <t>GRCh38.p13</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/000/001/405/GCA_000001405.28_GRCh38.p13/GCA_000001405.28_GRCh38.p13_protein.faa.gz</t>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCF/000/001/405/GCF_000001405.39_GRCh38.p13/GCF_000001405.39_GRCh38.p13_protein.faa.gz</t>
   </si>
   <si>
     <t>Homo sapiens.faa.gz</t>
@@ -130,7 +130,7 @@
     <t>ASM97006v1</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/000/970/065/GCA_000970065.1_ASM97006v1/GCA_000970065.1_ASM97006v1_protein.faa.gz</t>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCF/000/970/065/GCF_000970065.1_ASM97006v1/GCF_000970065.1_ASM97006v1_protein.faa.gz</t>
   </si>
   <si>
     <t>Methanosarcina barkeri.faa.gz</t>
@@ -157,7 +157,7 @@
     <t>ASM1292v1</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/000/012/925/GCA_000012925.1_ASM1292v1/GCA_000012925.1_ASM1292v1_protein.faa.gz</t>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCF/000/012/925/GCF_000012925.1_ASM1292v1/GCF_000012925.1_ASM1292v1_protein.faa.gz</t>
   </si>
   <si>
     <t>Geobacter metallireducens.faa.gz</t>
@@ -181,7 +181,7 @@
     <t>GCA_900002375</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/900/002/375/GCA_900002375.2_GCA_900002375/GCA_900002375.2_GCA_900002375_protein.faa.gz</t>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCF/900/002/375/GCF_900002375.2_GCA_900002375/GCF_900002375.2_GCA_900002375_protein.faa.gz</t>
   </si>
   <si>
     <t>Plasmodium berghei.faa.gz</t>
@@ -208,7 +208,7 @@
     <t>PcynB_1.0</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/000/321/355/GCA_000321355.1_PcynB_1.0/GCA_000321355.1_PcynB_1.0_protein.faa.gz</t>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCF/000/321/355/GCF_000321355.1_PcynB_1.0/GCF_000321355.1_PcynB_1.0_protein.faa.gz</t>
   </si>
   <si>
     <t>Plasmodium cynomolgi.faa.gz</t>
@@ -235,7 +235,7 @@
     <t>GCA_000002765</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/000/002/765/GCA_000002765.3_GCA_000002765/GCA_000002765.3_GCA_000002765_protein.faa.gz</t>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCF/000/002/765/GCF_000002765.5_GCA_000002765/GCF_000002765.5_GCA_000002765_protein.faa.gz</t>
   </si>
   <si>
     <t>Plasmodium falciparum.faa.gz</t>
@@ -262,7 +262,7 @@
     <t>GCA_000006355.2</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/000/006/355/GCA_000006355.3_GCA_000006355.2/GCA_000006355.3_GCA_000006355.2_protein.faa.gz</t>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCF/000/006/355/GCF_000006355.2_GCA_000006355.2/GCF_000006355.2_GCA_000006355.2_protein.faa.gz</t>
   </si>
   <si>
     <t>Plasmodium knowlesi.faa.gz</t>
@@ -289,7 +289,7 @@
     <t>ASM241v2</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/000/002/415/GCA_000002415.2_ASM241v2/GCA_000002415.2_ASM241v2_protein.faa.gz</t>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCF/000/002/415/GCF_000002415.2_ASM241v2/GCF_000002415.2_ASM241v2_protein.faa.gz</t>
   </si>
   <si>
     <t>Plasmodium vivax.faa.gz</t>
@@ -316,7 +316,7 @@
     <t>CriGri_1.0</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/000/223/135/GCA_000223135.1_CriGri_1.0/GCA_000223135.1_CriGri_1.0_protein.faa.gz</t>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCF/000/223/135/GCF_000223135.1_CriGri_1.0/GCF_000223135.1_CriGri_1.0_protein.faa.gz</t>
   </si>
   <si>
     <t>Cricetulus griseus.faa.gz</t>
@@ -343,7 +343,7 @@
     <t>ASM211692v1</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/002/116/925/GCA_002116925.1_ASM211692v1/GCA_002116925.1_ASM211692v1_protein.faa.gz</t>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCF/002/116/925/GCF_002116925.1_ASM211692v1/GCF_002116925.1_ASM211692v1_protein.faa.gz</t>
   </si>
   <si>
     <t>Acinetobacter baumannii.faa.gz</t>
@@ -370,7 +370,7 @@
     <t>ASM200788v1</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/002/007/885/GCA_002007885.1_ASM200788v1/GCA_002007885.1_ASM200788v1_protein.faa.gz</t>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCF/002/007/885/GCF_002007885.1_ASM200788v1/GCF_002007885.1_ASM200788v1_protein.faa.gz</t>
   </si>
   <si>
     <t>Clostridioides difficile.faa.gz</t>
@@ -397,7 +397,7 @@
     <t>ASM19595v2</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/000/195/955/GCA_000195955.2_ASM19595v2/GCA_000195955.2_ASM19595v2_protein.faa.gz</t>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCF/000/195/955/GCF_000195955.2_ASM19595v2/GCF_000195955.2_ASM19595v2_protein.faa.gz</t>
   </si>
   <si>
     <t>Mycobacterium tuberculosis.faa.gz</t>
@@ -424,7 +424,7 @@
     <t>ASM14368v1</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/000/143/685/GCA_000143685.1_ASM14368v1/GCA_000143685.1_ASM14368v1_protein.faa.gz</t>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCF/000/143/685/GCF_000143685.1_ASM14368v1/GCF_000143685.1_ASM14368v1_protein.faa.gz</t>
   </si>
   <si>
     <t>Clostridium ljungdahlii.faa.gz</t>
@@ -451,7 +451,7 @@
     <t>ASM20906v1</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/000/209/065/GCA_000209065.1_ASM20906v1/GCA_000209065.1_ASM20906v1_protein.faa.gz</t>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCF/000/209/065/GCF_000209065.1_ASM20906v1/GCF_000209065.1_ASM20906v1_protein.faa.gz</t>
   </si>
   <si>
     <t>Trypanosoma cruzi.faa.gz</t>
@@ -478,7 +478,7 @@
     <t>ASM22455v1</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/000/224/555/GCA_000224555.1_ASM22455v1/GCA_000224555.1_ASM22455v1_protein.faa.gz</t>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCF/000/224/555/GCF_000224555.1_ASM22455v1/GCF_000224555.1_ASM22455v1_protein.faa.gz</t>
   </si>
   <si>
     <t>Helicobacter pylori.faa.gz</t>
@@ -505,7 +505,7 @@
     <t>ASM1252v1</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/000/012/525/GCA_000012525.1_ASM1252v1/GCA_000012525.1_ASM1252v1_protein.faa.gz</t>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCF/000/012/525/GCF_000012525.1_ASM1252v1/GCF_000012525.1_ASM1252v1_protein.faa.gz</t>
   </si>
   <si>
     <t>Synechococcus elongatus.faa.gz</t>
@@ -532,7 +532,7 @@
     <t>ASM41267v1</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/000/412/675/GCA_000412675.1_ASM41267v1/GCA_000412675.1_ASM41267v1_protein.faa.gz</t>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCF/000/412/675/GCF_000412675.1_ASM41267v1/GCF_000412675.1_ASM41267v1_protein.faa.gz</t>
   </si>
   <si>
     <t>Pseudomonas putida.faa.gz</t>
@@ -577,7 +577,7 @@
     <t>ASM15095v2</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/000/150/955/GCA_000150955.2_ASM15095v2/GCA_000150955.2_ASM15095v2_protein.faa.gz</t>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCF/000/150/955/GCF_000150955.2_ASM15095v2/GCF_000150955.2_ASM15095v2_protein.faa.gz</t>
   </si>
   <si>
     <t>Phaeodactylum tricornutum.faa.gz</t>
@@ -604,7 +604,7 @@
     <t>ASM23065v3</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/000/230/655/GCA_000230655.3_ASM23065v3/GCA_000230655.3_ASM23065v3_protein.faa.gz</t>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCF/000/230/655/GCF_000230655.2_ASM23065v3/GCF_000230655.2_ASM23065v3_protein.faa.gz</t>
   </si>
   <si>
     <t>Thermotoga maritima.faa.gz</t>
@@ -628,7 +628,7 @@
     <t>GRCm39</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/000/001/635/GCA_000001635.9_GRCm39/GCA_000001635.9_GRCm39_protein.faa.gz</t>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCF/000/001/635/GCF_000001635.27_GRCm39/GCF_000001635.27_GRCm39_protein.faa.gz</t>
   </si>
   <si>
     <t>Mus musculus.faa.gz</t>
@@ -655,7 +655,7 @@
     <t>R64</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/000/146/045/GCA_000146045.2_R64/GCA_000146045.2_R64_protein.faa.gz</t>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCF/000/146/045/GCF_000146045.2_R64/GCF_000146045.2_R64_protein.faa.gz</t>
   </si>
   <si>
     <t>Saccharomyces cerevisiae.faa.gz</t>
@@ -682,7 +682,7 @@
     <t>ASM46895v1</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/000/468/955/GCA_000468955.1_ASM46895v1/GCA_000468955.1_ASM46895v1_protein.faa.gz</t>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCF/000/468/955/GCF_000468955.1_ASM46895v1/GCF_000468955.1_ASM46895v1_protein.faa.gz</t>
   </si>
   <si>
     <t>Lactococcus lactis subsp. cremoris.faa.gz</t>
@@ -739,7 +739,7 @@
     <t>ASM692v2</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/000/006/925/GCA_000006925.2_ASM692v2/GCA_000006925.2_ASM692v2_protein.faa.gz</t>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCF/000/006/925/GCF_000006925.2_ASM692v2/GCF_000006925.2_ASM692v2_protein.faa.gz</t>
   </si>
   <si>
     <t>Shigella flexneri.faa.gz</t>
@@ -766,7 +766,7 @@
     <t>ASM1342v1</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/000/013/425/GCA_000013425.1_ASM1342v1/GCA_000013425.1_ASM1342v1_protein.faa.gz</t>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCF/000/013/425/GCF_000013425.1_ASM1342v1/GCF_000013425.1_ASM1342v1_protein.faa.gz</t>
   </si>
   <si>
     <t>Staphylococcus aureus subsp. aureus.faa.gz</t>
@@ -793,7 +793,7 @@
     <t>ASM357230v1</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/003/572/305/GCA_003572305.1_ASM357230v1/GCA_003572305.1_ASM357230v1_protein.faa.gz</t>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCF/003/572/305/GCF_003572305.1_ASM357230v1/GCF_003572305.1_ASM357230v1_protein.faa.gz</t>
   </si>
   <si>
     <t>Shigella boydii.faa.gz</t>
@@ -820,7 +820,7 @@
     <t>ASM1547559v1</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/015/475/595/GCA_015475595.1_ASM1547559v1/GCA_015475595.1_ASM1547559v1_protein.faa.gz</t>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCF/015/475/595/GCF_015475595.1_ASM1547559v1/GCF_015475595.1_ASM1547559v1_protein.faa.gz</t>
   </si>
   <si>
     <t>Shigella dysenteriae.faa.gz</t>
@@ -847,7 +847,7 @@
     <t>ASM224748v1</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/002/247/485/GCA_002247485.1_ASM224748v1/GCA_002247485.1_ASM224748v1_protein.faa.gz</t>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCF/002/247/485/GCF_002247485.1_ASM224748v1/GCF_002247485.1_ASM224748v1_protein.faa.gz</t>
   </si>
   <si>
     <t>Shigella sonnei.faa.gz</t>
@@ -874,7 +874,7 @@
     <t>ASM24018v2</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/000/240/185/GCA_000240185.2_ASM24018v2/GCA_000240185.2_ASM24018v2_protein.faa.gz</t>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCF/000/240/185/GCF_000240185.1_ASM24018v2/GCF_000240185.1_ASM24018v2_protein.faa.gz</t>
   </si>
   <si>
     <t>Klebsiella pneumoniae subsp. pneumoniae.faa.gz</t>
@@ -901,7 +901,7 @@
     <t>ASM904v1</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/000/009/045/GCA_000009045.1_ASM904v1/GCA_000009045.1_ASM904v1_protein.faa.gz</t>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCF/000/009/045/GCF_000009045.1_ASM904v1/GCF_000009045.1_ASM904v1_protein.faa.gz</t>
   </si>
   <si>
     <t>Bacillus subtilis subsp. subtilis.faa.gz</t>
@@ -937,19 +937,16 @@
     <t>ASM694v2</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/000/006/945/GCA_000006945.2_ASM694v2/GCA_000006945.2_ASM694v2_protein.faa.gz</t>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/genomes/all/GCF/000/006/945/GCF_000006945.2_ASM694v2/GCF_000006945.2_ASM694v2_protein.faa.gz</t>
   </si>
   <si>
     <t>Salmonella enterica subsp. enterica.faa.gz</t>
   </si>
   <si>
-    <t>https://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/011/392/055/GCA_011392055.1_ASM1139205v1/</t>
-  </si>
-  <si>
-    <t>https://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/000/222/975/GCA_000222975.1_ASM22297v1/</t>
-  </si>
-  <si>
-    <t>https://ftp.ncbi.nlm.nih.gov/genomes/all/GCA/000/002/595/GCA_000002595.2_v3.0/</t>
+    <t>https://ftp.ncbi.nlm.nih.gov/genomes/all/GCF/011/392/055/GCF_011392055.1_ASM1139205v1/</t>
+  </si>
+  <si>
+    <t>https://ftp.ncbi.nlm.nih.gov/genomes/all/GCF/000/222/975/GCF_000222975.1_ASM22297v1/</t>
   </si>
 </sst>
 </file>
@@ -1314,8 +1311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30:L31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2287,7 +2284,7 @@
         <v>227</v>
       </c>
       <c r="L26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
@@ -2313,13 +2310,13 @@
         <v>226</v>
       </c>
       <c r="J27" t="s">
-        <v>309</v>
+        <v>176</v>
       </c>
       <c r="K27" t="s">
         <v>231</v>
       </c>
       <c r="L27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>